<commit_message>
aanpassing tabellen voor extra timesteps
</commit_message>
<xml_diff>
--- a/final_ass_time_changed/data/hydrology/werklijn_params.xlsx
+++ b/final_ass_time_changed/data/hydrology/werklijn_params.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27804"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_E058001F0E200105F4C507A5A33D7C08DFD71720" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD2BD40-61BE-4B01-9CDA-6E085D2B83AF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -33,8 +50,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,7 +84,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -75,14 +92,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -120,7 +140,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -192,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -365,16 +385,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -402,31 +422,67 @@
         <v>5893.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
+        <f>(A2+A4)/2</f>
+        <v>3508.5</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:D3" si="0">(B2+B4)/2</f>
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>1569.3691435000001</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>5929.1962025000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>7017</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1517.58187</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>5965.0924050000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <f>(A4+A6)/2</f>
+        <v>8933.5</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:D5" si="1">(B4+B6)/2</f>
+        <v>13.5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1417.0181480000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>6288.7945395000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>10850</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>1316.454426</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>6612.496674</v>
       </c>
     </row>
@@ -436,24 +492,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>